<commit_message>
updated excel file with run results
</commit_message>
<xml_diff>
--- a/projects/language-translation/abstract_translation_results.xlsx
+++ b/projects/language-translation/abstract_translation_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/otrejo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/otrejo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E0254C9-4D43-6148-9211-F2B47CAE66C4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A1B05E-9B8D-ED4E-AE57-68055880690C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="5560" windowWidth="28040" windowHeight="11500" xr2:uid="{22E81C88-8AE2-C94C-B95B-37C729B477BA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Epochs</t>
   </si>
@@ -131,6 +131,24 @@
   </si>
   <si>
     <t>Original_title</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>cleaner</t>
+  </si>
+  <si>
+    <t>the role of the earth in the solar system</t>
+  </si>
+  <si>
+    <t>the precis imag of the earth of the earth</t>
+  </si>
+  <si>
+    <t>first space imag from a dslr object from the new planet &lt;EOS&gt;</t>
   </si>
 </sst>
 </file>
@@ -491,21 +509,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F18A6D-B2FB-784B-B2CF-704A699185F3}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="76.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="79.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="76.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,13 +543,16 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12</v>
       </c>
@@ -551,13 +572,16 @@
         <v>2.4946999999999999</v>
       </c>
       <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12</v>
       </c>
@@ -577,13 +601,16 @@
         <v>2.6783999999999999</v>
       </c>
       <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>48</v>
       </c>
@@ -603,13 +630,16 @@
         <v>0.94120000000000004</v>
       </c>
       <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>48</v>
       </c>
@@ -629,13 +659,16 @@
         <v>1.3460000000000001</v>
       </c>
       <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>48</v>
       </c>
@@ -655,13 +688,16 @@
         <v>1.8443000000000001</v>
       </c>
       <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>48</v>
       </c>
@@ -681,14 +717,106 @@
         <v>1.8813</v>
       </c>
       <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
         <v>12</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>0.44919999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.39879999999999999</v>
+      </c>
+      <c r="F8">
+        <v>2.6705999999999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>128</v>
+      </c>
+      <c r="D9">
+        <v>0.51910000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.46089999999999998</v>
+      </c>
+      <c r="F9">
+        <v>1.7501</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f>48*4</f>
+        <v>192</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.45119999999999999</v>
+      </c>
+      <c r="F10">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>